<commit_message>
Changes made on 15/09/2024 at 20:05:45,05 from PC Home
</commit_message>
<xml_diff>
--- a/Courses roadmap.xlsx
+++ b/Courses roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer's Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AA74D1-51F7-4E92-9BA6-17251DAD7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CD5207-1FA0-402B-A84A-D8609C8A70EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Modern HTML &amp; CSS From The Beginning 2.0</t>
   </si>
@@ -51,16 +51,10 @@
     <t>CSS Basics</t>
   </si>
   <si>
-    <t>Box Model &amp; Positioning</t>
-  </si>
-  <si>
     <t>HTML Form &amp; Input Elements</t>
   </si>
   <si>
     <t>More HTML Elements</t>
-  </si>
-  <si>
-    <t>Flexbox</t>
   </si>
 </sst>
 </file>
@@ -90,7 +84,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,7 +104,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -151,8 +145,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +512,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -533,31 +527,33 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>

</xml_diff>

<commit_message>
Changes made on 07/10/2024 at  7:03:33,11 from PC Home
</commit_message>
<xml_diff>
--- a/Courses roadmap.xlsx
+++ b/Courses roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer's Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CD5207-1FA0-402B-A84A-D8609C8A70EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2F0A5E-30F6-463E-BBD9-92134478C7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Modern HTML &amp; CSS From The Beginning 2.0</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>More HTML Elements</t>
+  </si>
+  <si>
+    <t>Fonts in css</t>
   </si>
 </sst>
 </file>
@@ -427,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +496,7 @@
         <v>45538</v>
       </c>
       <c r="Q1" s="2">
-        <v>45539</v>
+        <v>45569</v>
       </c>
       <c r="R1" s="2">
         <v>45540</v>
@@ -554,7 +557,9 @@
       <c r="P2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>

</xml_diff>